<commit_message>
Apogée : mise à jour des données de septembre 2018
</commit_message>
<xml_diff>
--- a/data-raw/Individu.xlsx
+++ b/data-raw/Individu.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1146" uniqueCount="658">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1144" uniqueCount="656">
   <si>
     <t>Bac ou équivalence (code)</t>
   </si>
@@ -1662,12 +1662,6 @@
   </si>
   <si>
     <t>ZAMBIEN(NE)</t>
-  </si>
-  <si>
-    <t>347</t>
-  </si>
-  <si>
-    <t>BOTSWANAIS(E)</t>
   </si>
   <si>
     <t>348</t>
@@ -5323,7 +5317,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C183"/>
+  <dimension ref="A1:C182"/>
   <sheetViews>
     <sheetView rightToLeft="0" workbookViewId="0"/>
   </sheetViews>
@@ -6668,15 +6662,15 @@
         <v>630</v>
       </c>
       <c r="C168" s="4" t="s">
-        <v>631</v>
+        <v>589</v>
       </c>
     </row>
     <row r="169" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B169" s="3" t="s">
+        <v>631</v>
+      </c>
+      <c r="C169" s="3" t="s">
         <v>632</v>
-      </c>
-      <c r="C169" s="3" t="s">
-        <v>591</v>
       </c>
     </row>
     <row r="170" s="1" customFormat="1" ht="19.7321" customHeight="1">
@@ -6772,18 +6766,10 @@
         <v>655</v>
       </c>
       <c r="C181" s="3" t="s">
-        <v>656</v>
-      </c>
-    </row>
-    <row r="182" s="1" customFormat="1" ht="19.7321" customHeight="1">
-      <c r="B182" s="4" t="s">
-        <v>657</v>
-      </c>
-      <c r="C182" s="4" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="183" s="1" customFormat="1" ht="28.7982" customHeight="1"/>
+        <v>652</v>
+      </c>
+    </row>
+    <row r="182" s="1" customFormat="1" ht="28.7982" customHeight="1"/>
   </sheetData>
   <pageSetup paperSize="9" scale="100" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>

</xml_diff>

<commit_message>
Apogée : mise à jour 4/10/18
</commit_message>
<xml_diff>
--- a/data-raw/Individu.xlsx
+++ b/data-raw/Individu.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1144" uniqueCount="656">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1146" uniqueCount="658">
   <si>
     <t>Bac ou équivalence (code)</t>
   </si>
@@ -1890,6 +1890,12 @@
   </si>
   <si>
     <t>GUYANAIS(E)</t>
+  </si>
+  <si>
+    <t>429</t>
+  </si>
+  <si>
+    <t>BELIZE</t>
   </si>
   <si>
     <t>435</t>
@@ -5317,7 +5323,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C182"/>
+  <dimension ref="A1:C183"/>
   <sheetViews>
     <sheetView rightToLeft="0" workbookViewId="0"/>
   </sheetViews>
@@ -6662,15 +6668,15 @@
         <v>630</v>
       </c>
       <c r="C168" s="4" t="s">
-        <v>589</v>
+        <v>631</v>
       </c>
     </row>
     <row r="169" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B169" s="3" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="C169" s="3" t="s">
-        <v>632</v>
+        <v>589</v>
       </c>
     </row>
     <row r="170" s="1" customFormat="1" ht="19.7321" customHeight="1">
@@ -6766,10 +6772,18 @@
         <v>655</v>
       </c>
       <c r="C181" s="3" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="182" s="1" customFormat="1" ht="28.7982" customHeight="1"/>
+        <v>656</v>
+      </c>
+    </row>
+    <row r="182" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B182" s="4" t="s">
+        <v>657</v>
+      </c>
+      <c r="C182" s="4" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="183" s="1" customFormat="1" ht="28.7982" customHeight="1"/>
   </sheetData>
   <pageSetup paperSize="9" scale="100" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>

</xml_diff>

<commit_message>
Mise à jour apogée 10/05/2019
</commit_message>
<xml_diff>
--- a/data-raw/Individu.xlsx
+++ b/data-raw/Individu.xlsx
@@ -7,12 +7,13 @@
     <sheet name="Bac - nomenclature" sheetId="3" r:id="rId3"/>
     <sheet name="Type établissement" sheetId="4" r:id="rId4"/>
     <sheet name="Nationalité" sheetId="5" r:id="rId5"/>
+    <sheet name="Situation_annee_precedente" sheetId="6" r:id="rId6"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1146" uniqueCount="658">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1186" uniqueCount="685">
   <si>
     <t>Bac ou équivalence (code)</t>
   </si>
@@ -1986,6 +1987,87 @@
   </si>
   <si>
     <t>999</t>
+  </si>
+  <si>
+    <t>Situation année précédente (code)</t>
+  </si>
+  <si>
+    <t>Situation année précédente (lib.)</t>
+  </si>
+  <si>
+    <t>Enseignement secondaire (y compris par correspondance)</t>
+  </si>
+  <si>
+    <t>BTS</t>
+  </si>
+  <si>
+    <t>CPGE (non inscrit à l'université)</t>
+  </si>
+  <si>
+    <t>Ecole d'ingénieur (universitaire ou non)</t>
+  </si>
+  <si>
+    <t>Université (hors IUT, IUFM, Ecole d'ingénieur universitaire)</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>Ecole de MANAGEMENT (commerce, gestion)</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>Autre établissement SISE</t>
+  </si>
+  <si>
+    <t>Etablissement (hors université) préparant aux concours paramédicaux</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>ESPE</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Etablissement étranger d'enseignement supérieur ou secondaire</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>Etab Etranger ens secondaire</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>Etab etranger ens supérieur</t>
+  </si>
+  <si>
+    <t>Autre établissement ou cursus (hors secondaire, STS, Ingénieur, CPGE, Universitaire, IUT, IUFM, établissements préparant</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>Non scolarisé l'année précédente et jamais entré dans l'enseignement supérieur (prise d'étude différée)</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>Non scolarisé l'année précédente mais précédemment entré dans l'enseignement supérieur, universitaire ou non (reprise d'</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>Instituts catholiques</t>
   </si>
 </sst>
 </file>
@@ -6773,4 +6855,181 @@
   <pageSetup paperSize="9" scale="100" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C22"/>
+  <cols>
+    <col min="1" max="1" width="15.9715986666667" customWidth="1"/>
+    <col min="2" max="3" width="10.7163133333333" customWidth="1"/>
+    <col min="4" max="4" width="4.67767866666667" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" ht="14.3991" customHeight="1"/>
+    <row r="2" s="1" customFormat="1" ht="23.9985" customHeight="1">
+      <c r="B2" s="2" t="s">
+        <v>658</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="3" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="4" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="5" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="6" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B6" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="7" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B7" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="8" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B8" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="9" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B9" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="10" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B10" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="11" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B11" s="3" t="s">
+        <v>665</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="12" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B12" s="4" t="s">
+        <v>667</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="13" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B13" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="14" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B14" s="4" t="s">
+        <v>670</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="15" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B15" s="3" t="s">
+        <v>672</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="16" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B16" s="4" t="s">
+        <v>674</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="17" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B17" s="3" t="s">
+        <v>676</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="18" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B18" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="19" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B19" s="3" t="s">
+        <v>679</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="20" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B20" s="4" t="s">
+        <v>681</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="21" s="1" customFormat="1" ht="19.7321" customHeight="1">
+      <c r="B21" s="3" t="s">
+        <v>683</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="22" s="1" customFormat="1" ht="28.7982" customHeight="1"/>
+  </sheetData>
+  <pageSetup paperSize="9" scale="100" orientation="portrait"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
 </file>
</xml_diff>